<commit_message>
Testing doc, Matrix, Whitebox test case for mapping
Testing doc for MS04 and Matrix tickets have been updated according to MS04. Testcase code for mapping.c has been updated.
</commit_message>
<xml_diff>
--- a/Documents/Testing/Test Documents/Traceability Matrix NEW.xlsx
+++ b/Documents/Testing/Test Documents/Traceability Matrix NEW.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shsj0\Desktop\SFT_GROUP_PROJECT\Documents\Testing\Test Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB0E5D9-AFBE-4DE3-AA43-25B2E5316512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{585FD5BD-ECA0-4BDB-8A19-CF3255C4E15C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21150" xr2:uid="{55AD336A-B55A-431B-B962-6A6CD4943E33}"/>
+    <workbookView xWindow="6480" yWindow="3855" windowWidth="19470" windowHeight="15585" xr2:uid="{55AD336A-B55A-431B-B962-6A6CD4943E33}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
   <si>
     <t>S no.</t>
   </si>
@@ -101,9 +101,6 @@
     <t>Ending position check as 25 and Y</t>
   </si>
   <si>
-    <t xml:space="preserve">FAIL </t>
-  </si>
-  <si>
     <t>Open</t>
   </si>
   <si>
@@ -111,13 +108,98 @@
   </si>
   <si>
     <t>Def2</t>
+  </si>
+  <si>
+    <t>WB1</t>
+  </si>
+  <si>
+    <t>hasDestination</t>
+  </si>
+  <si>
+    <t>Overload</t>
+  </si>
+  <si>
+    <t>BixSizeExceed</t>
+  </si>
+  <si>
+    <t>ValidCargo</t>
+  </si>
+  <si>
+    <t>test_hasDestination();</t>
+  </si>
+  <si>
+    <t>test_isTruckOverloaded();</t>
+  </si>
+  <si>
+    <t>test_isBoxSizeExceeded();</t>
+  </si>
+  <si>
+    <t>test_validCargo();</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    shipment.destination.row = 5;
+    shipment.destination.col = 5;</t>
+  </si>
+  <si>
+    <t>Truck has destination</t>
+  </si>
+  <si>
+    <t>Truck overloaded</t>
+  </si>
+  <si>
+    <t>Box size checking</t>
+  </si>
+  <si>
+    <t>Cargo if valid</t>
+  </si>
+  <si>
+    <t>isTruckOverloaded(truck, ship);</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> float boxSize = 5.0;</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>Def3</t>
+  </si>
+  <si>
+    <t>Update</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PASS </t>
+  </si>
+  <si>
+    <t>Debugged and Closed on July 25</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> float boxSize = 0.5;</t>
+  </si>
+  <si>
+    <t>WB3</t>
+  </si>
+  <si>
+    <t>addRoute()</t>
+  </si>
+  <si>
+    <t>Testing add route in mapping</t>
+  </si>
+  <si>
+    <t>test_addRoute()</t>
+  </si>
+  <si>
+    <t>struct Route route = { 'X', 1, 1, 5, 'E' };</t>
+  </si>
+  <si>
+    <t>Def4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,6 +216,12 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -246,9 +334,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -267,14 +362,32 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -590,23 +703,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{108E63EF-5958-48C6-8336-44F660C2959D}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17:F19"/>
+      <selection activeCell="J20" sqref="J20:J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -634,354 +749,488 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="J1" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="5"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="8"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="9"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="4" t="s">
+      <c r="F4" s="6"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="5"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="8"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="9"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="4" t="s">
+      <c r="F7" s="6"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="I8" s="9" t="s">
+      <c r="G8" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="11" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="5"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="8"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="9"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="9"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="9"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="4" t="s">
+      <c r="F10" s="6"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="4"/>
+      <c r="J11" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>2</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="I14" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="9"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="9"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>2</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+    </row>
+    <row r="26" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="13">
+        <v>3</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="G26" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="H26" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="I26" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="J26" s="13"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="13"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="13"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="13"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="54">
-    <mergeCell ref="G23:G25"/>
-    <mergeCell ref="H23:H25"/>
-    <mergeCell ref="I23:I25"/>
-    <mergeCell ref="F23:F25"/>
+  <mergeCells count="75">
+    <mergeCell ref="F26:F28"/>
+    <mergeCell ref="H26:H28"/>
+    <mergeCell ref="I26:I28"/>
+    <mergeCell ref="J26:J28"/>
+    <mergeCell ref="G26:G28"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="E26:E28"/>
     <mergeCell ref="G14:G16"/>
     <mergeCell ref="H14:H16"/>
     <mergeCell ref="I14:I16"/>
     <mergeCell ref="G17:G19"/>
     <mergeCell ref="H17:H19"/>
     <mergeCell ref="I17:I19"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="G23:G25"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="I23:I25"/>
+    <mergeCell ref="F23:F25"/>
     <mergeCell ref="G20:G22"/>
     <mergeCell ref="H20:H22"/>
     <mergeCell ref="I20:I22"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="E23:E25"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="C23:C25"/>
     <mergeCell ref="D14:D16"/>
     <mergeCell ref="D17:D19"/>
     <mergeCell ref="D20:D22"/>
     <mergeCell ref="D23:D25"/>
     <mergeCell ref="E14:E16"/>
     <mergeCell ref="E17:E19"/>
-    <mergeCell ref="E20:E22"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="C14:C25"/>
-    <mergeCell ref="E23:E25"/>
-    <mergeCell ref="F14:F16"/>
-    <mergeCell ref="F17:F19"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="I5:I7"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="G5:G7"/>
-    <mergeCell ref="F5:F7"/>
     <mergeCell ref="I2:I4"/>
     <mergeCell ref="H2:H4"/>
     <mergeCell ref="G2:G4"/>
@@ -992,6 +1241,12 @@
     <mergeCell ref="F11:F13"/>
     <mergeCell ref="H8:H10"/>
     <mergeCell ref="I8:I10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="I5:I7"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="G5:G7"/>
+    <mergeCell ref="F5:F7"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="C2:C13"/>
@@ -1003,6 +1258,14 @@
     <mergeCell ref="D5:D7"/>
     <mergeCell ref="D8:D10"/>
     <mergeCell ref="D11:D13"/>
+    <mergeCell ref="J8:J10"/>
+    <mergeCell ref="J2:J4"/>
+    <mergeCell ref="J5:J7"/>
+    <mergeCell ref="J23:J25"/>
+    <mergeCell ref="J20:J22"/>
+    <mergeCell ref="J17:J19"/>
+    <mergeCell ref="J14:J16"/>
+    <mergeCell ref="J11:J13"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update for Ms06 submission
</commit_message>
<xml_diff>
--- a/Documents/Testing/Test Documents/Traceability Matrix NEW.xlsx
+++ b/Documents/Testing/Test Documents/Traceability Matrix NEW.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shsj0\Desktop\SFT_GROUP_PROJECT\Documents\Testing\Test Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sangjunelee/Desktop/Study/SFT - Seneca/SFT GROUP/SFT_GROUP_PROJECT/Documents/Testing/Test Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B476126-9B95-45EA-9FD6-9347B2E0DF7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E2D1BF0-0E26-CA40-9C81-39EC1438D822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22575" yWindow="2940" windowWidth="19470" windowHeight="15585" xr2:uid="{55AD336A-B55A-431B-B962-6A6CD4943E33}"/>
+    <workbookView xWindow="-7180" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{55AD336A-B55A-431B-B962-6A6CD4943E33}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="61">
   <si>
     <t>S no.</t>
   </si>
@@ -205,6 +205,21 @@
   </si>
   <si>
     <t>INT1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAIL </t>
+  </si>
+  <si>
+    <t>Def6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acceptance Testing pass for all as user perspective </t>
+  </si>
+  <si>
+    <t>ACT1</t>
+  </si>
+  <si>
+    <t>Project and Jira updated</t>
   </si>
 </sst>
 </file>
@@ -239,7 +254,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -258,8 +273,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -336,25 +357,169 @@
         <color indexed="64"/>
       </diagonal>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="1" diagonalDown="1">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal style="thin">
+        <color indexed="64"/>
+      </diagonal>
+    </border>
+    <border diagonalUp="1" diagonalDown="1">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal style="thin">
+        <color indexed="64"/>
+      </diagonal>
+    </border>
+    <border diagonalUp="1" diagonalDown="1">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal style="thin">
+        <color indexed="64"/>
+      </diagonal>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -365,28 +530,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -703,25 +898,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{108E63EF-5958-48C6-8336-44F660C2959D}">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -753,207 +948,207 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="16"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="7"/>
       <c r="F3" s="13"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="16"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="7"/>
       <c r="F4" s="13"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="10" t="s">
+      <c r="G4" s="12"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="16"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="7"/>
       <c r="F6" s="13"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="16"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="7"/>
       <c r="F7" s="13"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="10" t="s">
+      <c r="G7" s="12"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="7" t="s">
         <v>15</v>
       </c>
       <c r="F8" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="5"/>
-      <c r="J8" s="16" t="s">
+      <c r="I8" s="6"/>
+      <c r="J8" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="16"/>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="7"/>
       <c r="F9" s="13"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="16"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="16"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="7"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="7"/>
       <c r="F10" s="13"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="16"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="10" t="s">
+      <c r="G10" s="4"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="7"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="7" t="s">
         <v>15</v>
       </c>
       <c r="F11" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H11" s="14" t="s">
+      <c r="H11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I11" s="5"/>
-      <c r="J11" s="16" t="s">
+      <c r="I11" s="6"/>
+      <c r="J11" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="16"/>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="7"/>
       <c r="F12" s="13"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="16"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="16"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="7"/>
       <c r="F13" s="13"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="16"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
+      <c r="G13" s="4"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="8">
         <v>2</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E14" s="3" t="s">
@@ -962,180 +1157,180 @@
       <c r="F14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="G14" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H14" s="17" t="s">
+      <c r="H14" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="I14" s="5"/>
-      <c r="J14" s="16" t="s">
+      <c r="I14" s="6"/>
+      <c r="J14" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="11"/>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="10"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="16"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="12"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="7"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="11"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="16"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7" t="s">
+      <c r="F16" s="8"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="7"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="9" t="s">
         <v>34</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G17" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="11"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="10"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="12"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="11"/>
       <c r="E19" s="3"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="7" t="s">
+      <c r="F19" s="8"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="9" t="s">
         <v>35</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="G20" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="11"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="10"/>
       <c r="E21" s="3"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="12"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="11"/>
       <c r="E22" s="3"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="7" t="s">
+      <c r="F22" s="8"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="9" t="s">
         <v>36</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F23" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="G23" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="11"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="10"/>
       <c r="E24" s="3"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="12"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="11"/>
       <c r="E25" s="3"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-    </row>
-    <row r="26" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F25" s="8"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+    </row>
+    <row r="26" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>3</v>
       </c>
@@ -1154,42 +1349,42 @@
       <c r="F26" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G26" s="15" t="s">
+      <c r="G26" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H26" s="17" t="s">
+      <c r="H26" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I26" s="5"/>
-      <c r="J26" s="16" t="s">
+      <c r="I26" s="6"/>
+      <c r="J26" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="16"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G27" s="4"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="7"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="16"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G28" s="4"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="7"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>4</v>
       </c>
@@ -1208,72 +1403,138 @@
       <c r="F29" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G29" s="15" t="s">
+      <c r="G29" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="H29" s="17" t="s">
+      <c r="H29" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="I29" s="5"/>
-      <c r="J29" s="16" t="s">
+      <c r="I29" s="6"/>
+      <c r="J29" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="16"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G30" s="18"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="7"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="16"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="7"/>
+    </row>
+    <row r="32" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="3">
+        <v>4</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I32" s="32"/>
+      <c r="J32" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="33"/>
+      <c r="J33" s="7"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="34"/>
+      <c r="J34" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="85">
-    <mergeCell ref="F29:F31"/>
-    <mergeCell ref="G29:G31"/>
-    <mergeCell ref="H29:H31"/>
-    <mergeCell ref="I29:I31"/>
-    <mergeCell ref="J29:J31"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="E29:E31"/>
-    <mergeCell ref="J8:J10"/>
-    <mergeCell ref="J2:J4"/>
-    <mergeCell ref="J5:J7"/>
-    <mergeCell ref="J23:J25"/>
-    <mergeCell ref="J20:J22"/>
-    <mergeCell ref="J17:J19"/>
-    <mergeCell ref="J14:J16"/>
-    <mergeCell ref="J11:J13"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="C2:C13"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="D11:D13"/>
+  <mergeCells count="92">
+    <mergeCell ref="G32:G34"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="I32:I34"/>
+    <mergeCell ref="J32:J34"/>
+    <mergeCell ref="C32:F34"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="F26:F28"/>
+    <mergeCell ref="H26:H28"/>
+    <mergeCell ref="I26:I28"/>
+    <mergeCell ref="J26:J28"/>
+    <mergeCell ref="G26:G28"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="I14:I16"/>
+    <mergeCell ref="G17:G19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="I17:I19"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="G23:G25"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="I23:I25"/>
+    <mergeCell ref="F23:F25"/>
+    <mergeCell ref="G20:G22"/>
+    <mergeCell ref="H20:H22"/>
+    <mergeCell ref="I20:I22"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="E23:E25"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="E17:E19"/>
     <mergeCell ref="I2:I4"/>
     <mergeCell ref="H2:H4"/>
     <mergeCell ref="G2:G4"/>
@@ -1290,46 +1551,35 @@
     <mergeCell ref="H5:H7"/>
     <mergeCell ref="G5:G7"/>
     <mergeCell ref="F5:F7"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="E23:E25"/>
-    <mergeCell ref="F14:F16"/>
-    <mergeCell ref="F17:F19"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="E14:E16"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="E20:E22"/>
-    <mergeCell ref="G23:G25"/>
-    <mergeCell ref="H23:H25"/>
-    <mergeCell ref="I23:I25"/>
-    <mergeCell ref="F23:F25"/>
-    <mergeCell ref="G20:G22"/>
-    <mergeCell ref="H20:H22"/>
-    <mergeCell ref="I20:I22"/>
-    <mergeCell ref="G14:G16"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="I14:I16"/>
-    <mergeCell ref="G17:G19"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="I17:I19"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="E26:E28"/>
-    <mergeCell ref="F26:F28"/>
-    <mergeCell ref="H26:H28"/>
-    <mergeCell ref="I26:I28"/>
-    <mergeCell ref="J26:J28"/>
-    <mergeCell ref="G26:G28"/>
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="C2:C13"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="J8:J10"/>
+    <mergeCell ref="J2:J4"/>
+    <mergeCell ref="J5:J7"/>
+    <mergeCell ref="J23:J25"/>
+    <mergeCell ref="J20:J22"/>
+    <mergeCell ref="J17:J19"/>
+    <mergeCell ref="J14:J16"/>
+    <mergeCell ref="J11:J13"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="F29:F31"/>
+    <mergeCell ref="G29:G31"/>
+    <mergeCell ref="H29:H31"/>
+    <mergeCell ref="I29:I31"/>
+    <mergeCell ref="J29:J31"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>